<commit_message>
All the documents from week 5
</commit_message>
<xml_diff>
--- a/Data_Sources/Hinnakiri.xlsx
+++ b/Data_Sources/Hinnakiri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opilane\Desktop\Andmetarkus,git\Andmetarkus\Timber AS\Timber-AS\Data_Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A697776-C2E1-45A3-828D-385B5822D117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F9EE89-68D8-4BF0-A83C-AE526453024E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{406E2A0B-FDA8-4376-9A38-F0A4084FE6A5}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Sortiment</t>
   </si>
   <si>
-    <t>Hind (€)</t>
-  </si>
-  <si>
     <t>Ma palk</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Jäätmed</t>
+  </si>
+  <si>
+    <t>Hind (€/tm)</t>
   </si>
 </sst>
 </file>
@@ -459,12 +459,13 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -472,12 +473,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>95</v>
@@ -485,7 +486,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>95</v>
@@ -493,7 +494,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>110</v>
@@ -501,7 +502,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>58</v>
@@ -509,7 +510,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>60</v>
@@ -517,7 +518,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>50</v>
@@ -525,7 +526,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>40</v>
@@ -533,7 +534,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
@@ -541,7 +542,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>40</v>
@@ -549,7 +550,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>40</v>
@@ -557,7 +558,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>35</v>
@@ -565,7 +566,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>64</v>
@@ -573,7 +574,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>64</v>
@@ -581,7 +582,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>62</v>
@@ -589,7 +590,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>62</v>
@@ -597,7 +598,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>50</v>
@@ -605,7 +606,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>50</v>
@@ -613,7 +614,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>39</v>
@@ -621,7 +622,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>

</xml_diff>